<commit_message>
manual publication corrections and image linkage
* corrected a lot of location clusters (only obvious errors such as spelling or latinizations
* established a link between records and actual first/title pages
</commit_message>
<xml_diff>
--- a/spatialnamesCorrections.xlsx
+++ b/spatialnamesCorrections.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/src/SBBrowse2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8244EACC-2ED8-1144-9875-6E3C67003917}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FA5307-2DBB-9243-86BA-947989AD6980}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2840" yWindow="460" windowWidth="25780" windowHeight="19600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5383" uniqueCount="3240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5595" uniqueCount="3292">
   <si>
     <t>SpatialClusterName</t>
   </si>
@@ -9740,6 +9740,162 @@
   </si>
   <si>
     <t>Burgund</t>
+  </si>
+  <si>
+    <t>Byzantinisches Reich</t>
+  </si>
+  <si>
+    <t>Cambridge, Massachusetts</t>
+  </si>
+  <si>
+    <t>Cap-d'Ail</t>
+  </si>
+  <si>
+    <t>Klagenfurt</t>
+  </si>
+  <si>
+    <t>Konstantinopel</t>
+  </si>
+  <si>
+    <t>Corbie</t>
+  </si>
+  <si>
+    <t>Cottbus</t>
+  </si>
+  <si>
+    <t>Kunersdorf</t>
+  </si>
+  <si>
+    <t>Danzig</t>
+  </si>
+  <si>
+    <t>Darjeeling</t>
+  </si>
+  <si>
+    <t>Densberg</t>
+  </si>
+  <si>
+    <t>Denver</t>
+  </si>
+  <si>
+    <t>Jarkata</t>
+  </si>
+  <si>
+    <t>Dortmund</t>
+  </si>
+  <si>
+    <t>Dresden</t>
+  </si>
+  <si>
+    <t>Duisburg</t>
+  </si>
+  <si>
+    <t>Dänemark</t>
+  </si>
+  <si>
+    <t>Ägypten</t>
+  </si>
+  <si>
+    <t>Erlangen</t>
+  </si>
+  <si>
+    <t>Frankfurt am Main</t>
+  </si>
+  <si>
+    <t>Frankreich</t>
+  </si>
+  <si>
+    <t>Göttingen</t>
+  </si>
+  <si>
+    <t>Heiligenstadt</t>
+  </si>
+  <si>
+    <t>Jerusalem</t>
+  </si>
+  <si>
+    <t>Kairo</t>
+  </si>
+  <si>
+    <t>Labaun</t>
+  </si>
+  <si>
+    <t>Liesborn</t>
+  </si>
+  <si>
+    <t>Locarno</t>
+  </si>
+  <si>
+    <t>Mönchen Gladbach</t>
+  </si>
+  <si>
+    <t>Madegaskar</t>
+  </si>
+  <si>
+    <t>Mur</t>
+  </si>
+  <si>
+    <t>Neapel</t>
+  </si>
+  <si>
+    <t>Neuruppin</t>
+  </si>
+  <si>
+    <t>Neubrandenburg</t>
+  </si>
+  <si>
+    <t>Ostfalen</t>
+  </si>
+  <si>
+    <t>Paderborn</t>
+  </si>
+  <si>
+    <t>Passau</t>
+  </si>
+  <si>
+    <t>Piešťany</t>
+  </si>
+  <si>
+    <t>Polen</t>
+  </si>
+  <si>
+    <t>Ratzeburg</t>
+  </si>
+  <si>
+    <t>Rheinfranken</t>
+  </si>
+  <si>
+    <t>Rostock</t>
+  </si>
+  <si>
+    <t>Timmendorfer Strand</t>
+  </si>
+  <si>
+    <t>Tokio</t>
+  </si>
+  <si>
+    <t>Vandœuvre-lès-Nancy</t>
+  </si>
+  <si>
+    <t>Wansleben</t>
+  </si>
+  <si>
+    <t>Weißenburg</t>
+  </si>
+  <si>
+    <t>Wernigerode</t>
+  </si>
+  <si>
+    <t>Wertheim</t>
+  </si>
+  <si>
+    <t>Westdeutschland</t>
+  </si>
+  <si>
+    <t>Wismar</t>
+  </si>
+  <si>
+    <t>Zweibrücken</t>
   </si>
 </sst>
 </file>
@@ -10143,8 +10299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2671"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A384" workbookViewId="0">
-      <selection activeCell="E384" sqref="E384"/>
+    <sheetView tabSelected="1" topLeftCell="A2635" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E2529" sqref="E2529"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18000,6 +18156,9 @@
       <c r="D387" t="s">
         <v>392</v>
       </c>
+      <c r="E387" t="s">
+        <v>3240</v>
+      </c>
       <c r="F387" t="b">
         <v>1</v>
       </c>
@@ -18489,7 +18648,7 @@
     </row>
     <row r="412" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A412" t="s">
-        <v>417</v>
+        <v>3241</v>
       </c>
       <c r="B412">
         <v>31</v>
@@ -18499,6 +18658,9 @@
       </c>
       <c r="D412" t="s">
         <v>417</v>
+      </c>
+      <c r="E412" t="s">
+        <v>3241</v>
       </c>
       <c r="F412" t="b">
         <v>1</v>
@@ -18620,6 +18782,9 @@
       <c r="D418" t="s">
         <v>2767</v>
       </c>
+      <c r="E418" t="s">
+        <v>424</v>
+      </c>
       <c r="F418" t="b">
         <v>0</v>
       </c>
@@ -18680,6 +18845,9 @@
       <c r="D421" t="s">
         <v>2768</v>
       </c>
+      <c r="E421" t="s">
+        <v>3242</v>
+      </c>
       <c r="F421" t="b">
         <v>0</v>
       </c>
@@ -18960,6 +19128,9 @@
       <c r="D435" t="s">
         <v>2769</v>
       </c>
+      <c r="E435" t="s">
+        <v>1125</v>
+      </c>
       <c r="F435" t="b">
         <v>0</v>
       </c>
@@ -18980,6 +19151,9 @@
       <c r="D436" t="s">
         <v>441</v>
       </c>
+      <c r="E436" t="s">
+        <v>1125</v>
+      </c>
       <c r="F436" t="b">
         <v>1</v>
       </c>
@@ -19960,6 +20134,9 @@
       <c r="D485" t="s">
         <v>2779</v>
       </c>
+      <c r="E485" t="s">
+        <v>3243</v>
+      </c>
       <c r="F485" t="b">
         <v>0</v>
       </c>
@@ -20120,6 +20297,9 @@
       <c r="D493" t="s">
         <v>2782</v>
       </c>
+      <c r="E493" t="s">
+        <v>1173</v>
+      </c>
       <c r="F493" t="b">
         <v>0</v>
       </c>
@@ -20400,6 +20580,9 @@
       <c r="D507" t="s">
         <v>2789</v>
       </c>
+      <c r="E507" t="s">
+        <v>3232</v>
+      </c>
       <c r="F507" t="b">
         <v>1</v>
       </c>
@@ -20420,6 +20603,9 @@
       <c r="D508" t="s">
         <v>2790</v>
       </c>
+      <c r="E508" t="s">
+        <v>3244</v>
+      </c>
       <c r="F508" t="b">
         <v>0</v>
       </c>
@@ -20480,6 +20666,9 @@
       <c r="D511" t="s">
         <v>516</v>
       </c>
+      <c r="E511" t="s">
+        <v>3245</v>
+      </c>
       <c r="F511" t="b">
         <v>0</v>
       </c>
@@ -20640,6 +20829,9 @@
       <c r="D519" t="s">
         <v>2791</v>
       </c>
+      <c r="E519" t="s">
+        <v>3246</v>
+      </c>
       <c r="F519" t="b">
         <v>0</v>
       </c>
@@ -20980,6 +21172,9 @@
       <c r="D536" t="s">
         <v>2794</v>
       </c>
+      <c r="E536" t="s">
+        <v>3247</v>
+      </c>
       <c r="F536" t="b">
         <v>0</v>
       </c>
@@ -21120,6 +21315,9 @@
       <c r="D543" t="s">
         <v>2795</v>
       </c>
+      <c r="E543" t="s">
+        <v>227</v>
+      </c>
       <c r="F543" t="b">
         <v>0</v>
       </c>
@@ -21140,6 +21338,9 @@
       <c r="D544" t="s">
         <v>549</v>
       </c>
+      <c r="E544" t="s">
+        <v>227</v>
+      </c>
       <c r="F544" t="b">
         <v>0</v>
       </c>
@@ -21360,6 +21561,9 @@
       <c r="D555" t="s">
         <v>2799</v>
       </c>
+      <c r="E555" t="s">
+        <v>3248</v>
+      </c>
       <c r="F555" t="b">
         <v>0</v>
       </c>
@@ -21400,6 +21604,9 @@
       <c r="D557" t="s">
         <v>562</v>
       </c>
+      <c r="E557" t="s">
+        <v>3249</v>
+      </c>
       <c r="F557" t="b">
         <v>0</v>
       </c>
@@ -21440,6 +21647,9 @@
       <c r="D559" t="s">
         <v>564</v>
       </c>
+      <c r="E559" t="s">
+        <v>563</v>
+      </c>
       <c r="F559" t="b">
         <v>1</v>
       </c>
@@ -21480,6 +21690,9 @@
       <c r="D561" t="s">
         <v>566</v>
       </c>
+      <c r="E561" t="s">
+        <v>3232</v>
+      </c>
       <c r="F561" t="b">
         <v>1</v>
       </c>
@@ -21660,6 +21873,9 @@
       <c r="D570" t="s">
         <v>575</v>
       </c>
+      <c r="E570" t="s">
+        <v>3250</v>
+      </c>
       <c r="F570" t="b">
         <v>1</v>
       </c>
@@ -21680,6 +21896,9 @@
       <c r="D571" t="s">
         <v>576</v>
       </c>
+      <c r="E571" t="s">
+        <v>3251</v>
+      </c>
       <c r="F571" t="b">
         <v>1</v>
       </c>
@@ -22120,6 +22339,9 @@
       <c r="D593" t="s">
         <v>598</v>
       </c>
+      <c r="E593" t="s">
+        <v>3232</v>
+      </c>
       <c r="F593" t="b">
         <v>0</v>
       </c>
@@ -22140,6 +22362,9 @@
       <c r="D594" t="s">
         <v>599</v>
       </c>
+      <c r="E594" t="s">
+        <v>3252</v>
+      </c>
       <c r="F594" t="b">
         <v>0</v>
       </c>
@@ -22320,6 +22545,9 @@
       <c r="D603" t="s">
         <v>608</v>
       </c>
+      <c r="E603" t="s">
+        <v>3232</v>
+      </c>
       <c r="F603" t="b">
         <v>0</v>
       </c>
@@ -22420,6 +22648,9 @@
       <c r="D608" t="s">
         <v>2813</v>
       </c>
+      <c r="E608" t="s">
+        <v>3253</v>
+      </c>
       <c r="F608" t="b">
         <v>0</v>
       </c>
@@ -22460,6 +22691,9 @@
       <c r="D610" t="s">
         <v>2814</v>
       </c>
+      <c r="E610" t="s">
+        <v>3254</v>
+      </c>
       <c r="F610" t="b">
         <v>1</v>
       </c>
@@ -22480,6 +22714,9 @@
       <c r="D611" t="s">
         <v>2815</v>
       </c>
+      <c r="E611" t="s">
+        <v>3254</v>
+      </c>
       <c r="F611" t="b">
         <v>1</v>
       </c>
@@ -22500,6 +22737,9 @@
       <c r="D612" t="s">
         <v>617</v>
       </c>
+      <c r="E612" t="s">
+        <v>3254</v>
+      </c>
       <c r="F612" t="b">
         <v>1</v>
       </c>
@@ -22520,6 +22760,9 @@
       <c r="D613" t="s">
         <v>618</v>
       </c>
+      <c r="E613" t="s">
+        <v>3254</v>
+      </c>
       <c r="F613" t="b">
         <v>1</v>
       </c>
@@ -22540,6 +22783,9 @@
       <c r="D614" t="s">
         <v>619</v>
       </c>
+      <c r="E614" t="s">
+        <v>3254</v>
+      </c>
       <c r="F614" t="b">
         <v>1</v>
       </c>
@@ -22560,6 +22806,9 @@
       <c r="D615" t="s">
         <v>620</v>
       </c>
+      <c r="E615" t="s">
+        <v>3254</v>
+      </c>
       <c r="F615" t="b">
         <v>1</v>
       </c>
@@ -22580,6 +22829,9 @@
       <c r="D616" t="s">
         <v>621</v>
       </c>
+      <c r="E616" t="s">
+        <v>3254</v>
+      </c>
       <c r="F616" t="b">
         <v>1</v>
       </c>
@@ -22600,6 +22852,9 @@
       <c r="D617" t="s">
         <v>2816</v>
       </c>
+      <c r="E617" t="s">
+        <v>3254</v>
+      </c>
       <c r="F617" t="b">
         <v>0</v>
       </c>
@@ -22700,6 +22955,9 @@
       <c r="D622" t="s">
         <v>627</v>
       </c>
+      <c r="E622" t="s">
+        <v>3255</v>
+      </c>
       <c r="F622" t="b">
         <v>1</v>
       </c>
@@ -22720,6 +22978,9 @@
       <c r="D623" t="s">
         <v>628</v>
       </c>
+      <c r="E623" t="s">
+        <v>3255</v>
+      </c>
       <c r="F623" t="b">
         <v>1</v>
       </c>
@@ -22740,6 +23001,9 @@
       <c r="D624" t="s">
         <v>2818</v>
       </c>
+      <c r="E624" t="s">
+        <v>3255</v>
+      </c>
       <c r="F624" t="b">
         <v>0</v>
       </c>
@@ -22820,6 +23084,9 @@
       <c r="D628" t="s">
         <v>633</v>
       </c>
+      <c r="E628" t="s">
+        <v>3256</v>
+      </c>
       <c r="F628" t="b">
         <v>0</v>
       </c>
@@ -22960,6 +23227,9 @@
       <c r="D635" t="s">
         <v>640</v>
       </c>
+      <c r="E635" t="s">
+        <v>639</v>
+      </c>
       <c r="F635" t="b">
         <v>1</v>
       </c>
@@ -22980,6 +23250,9 @@
       <c r="D636" t="s">
         <v>641</v>
       </c>
+      <c r="E636" t="s">
+        <v>3255</v>
+      </c>
       <c r="F636" t="b">
         <v>0</v>
       </c>
@@ -23240,6 +23513,9 @@
       <c r="D649" t="s">
         <v>654</v>
       </c>
+      <c r="E649" t="s">
+        <v>3257</v>
+      </c>
       <c r="F649" t="b">
         <v>0</v>
       </c>
@@ -23480,6 +23756,9 @@
       <c r="D661" t="s">
         <v>666</v>
       </c>
+      <c r="E661" t="s">
+        <v>3232</v>
+      </c>
       <c r="F661" t="b">
         <v>1</v>
       </c>
@@ -23500,6 +23779,9 @@
       <c r="D662" t="s">
         <v>667</v>
       </c>
+      <c r="E662" t="s">
+        <v>3232</v>
+      </c>
       <c r="F662" t="b">
         <v>0</v>
       </c>
@@ -23540,6 +23822,9 @@
       <c r="D664" t="s">
         <v>669</v>
       </c>
+      <c r="E664" t="s">
+        <v>668</v>
+      </c>
       <c r="F664" t="b">
         <v>1</v>
       </c>
@@ -23820,6 +24105,9 @@
       <c r="D678" t="s">
         <v>683</v>
       </c>
+      <c r="E678" t="s">
+        <v>3232</v>
+      </c>
       <c r="F678" t="b">
         <v>1</v>
       </c>
@@ -24060,6 +24348,9 @@
       <c r="D690" t="s">
         <v>2834</v>
       </c>
+      <c r="E690" t="s">
+        <v>3258</v>
+      </c>
       <c r="F690" t="b">
         <v>0</v>
       </c>
@@ -24080,6 +24371,9 @@
       <c r="D691" t="s">
         <v>696</v>
       </c>
+      <c r="E691" t="s">
+        <v>693</v>
+      </c>
       <c r="F691" t="b">
         <v>0</v>
       </c>
@@ -24100,6 +24394,9 @@
       <c r="D692" t="s">
         <v>697</v>
       </c>
+      <c r="E692" t="s">
+        <v>3232</v>
+      </c>
       <c r="F692" t="b">
         <v>1</v>
       </c>
@@ -24180,6 +24477,9 @@
       <c r="D696" t="s">
         <v>701</v>
       </c>
+      <c r="E696" t="s">
+        <v>700</v>
+      </c>
       <c r="F696" t="b">
         <v>0</v>
       </c>
@@ -24320,6 +24620,9 @@
       <c r="D703" t="s">
         <v>2835</v>
       </c>
+      <c r="E703" t="s">
+        <v>3232</v>
+      </c>
       <c r="F703" t="b">
         <v>1</v>
       </c>
@@ -24340,6 +24643,9 @@
       <c r="D704" t="s">
         <v>709</v>
       </c>
+      <c r="E704" t="s">
+        <v>702</v>
+      </c>
       <c r="F704" t="b">
         <v>0</v>
       </c>
@@ -24720,6 +25026,9 @@
       <c r="D723" t="s">
         <v>2836</v>
       </c>
+      <c r="E723" t="s">
+        <v>3232</v>
+      </c>
       <c r="F723" t="b">
         <v>0</v>
       </c>
@@ -24740,6 +25049,9 @@
       <c r="D724" t="s">
         <v>729</v>
       </c>
+      <c r="E724" t="s">
+        <v>739</v>
+      </c>
       <c r="F724" t="b">
         <v>0</v>
       </c>
@@ -24920,6 +25232,9 @@
       <c r="D733" t="s">
         <v>738</v>
       </c>
+      <c r="E733" t="s">
+        <v>739</v>
+      </c>
       <c r="F733" t="b">
         <v>0</v>
       </c>
@@ -24940,6 +25255,9 @@
       <c r="D734" t="s">
         <v>2838</v>
       </c>
+      <c r="E734" t="s">
+        <v>739</v>
+      </c>
       <c r="F734" t="b">
         <v>0</v>
       </c>
@@ -25180,6 +25498,9 @@
       <c r="D746" t="s">
         <v>2841</v>
       </c>
+      <c r="E746" t="s">
+        <v>3259</v>
+      </c>
       <c r="F746" t="b">
         <v>1</v>
       </c>
@@ -25280,6 +25601,9 @@
       <c r="D751" t="s">
         <v>2844</v>
       </c>
+      <c r="E751" t="s">
+        <v>3260</v>
+      </c>
       <c r="F751" t="b">
         <v>0</v>
       </c>
@@ -25800,6 +26124,9 @@
       <c r="D777" t="s">
         <v>782</v>
       </c>
+      <c r="E777" t="s">
+        <v>3232</v>
+      </c>
       <c r="F777" t="b">
         <v>1</v>
       </c>
@@ -27820,6 +28147,9 @@
       <c r="D878" t="s">
         <v>2872</v>
       </c>
+      <c r="E878" t="s">
+        <v>227</v>
+      </c>
       <c r="F878" t="b">
         <v>1</v>
       </c>
@@ -28240,6 +28570,9 @@
       <c r="D899" t="s">
         <v>904</v>
       </c>
+      <c r="E899" t="s">
+        <v>905</v>
+      </c>
       <c r="F899" t="b">
         <v>0</v>
       </c>
@@ -28300,6 +28633,9 @@
       <c r="D902" t="s">
         <v>2880</v>
       </c>
+      <c r="E902" t="s">
+        <v>3261</v>
+      </c>
       <c r="F902" t="b">
         <v>0</v>
       </c>
@@ -28400,6 +28736,9 @@
       <c r="D907" t="s">
         <v>912</v>
       </c>
+      <c r="E907" t="s">
+        <v>3232</v>
+      </c>
       <c r="F907" t="b">
         <v>0</v>
       </c>
@@ -28420,6 +28759,9 @@
       <c r="D908" t="s">
         <v>2882</v>
       </c>
+      <c r="E908" t="s">
+        <v>913</v>
+      </c>
       <c r="F908" t="b">
         <v>0</v>
       </c>
@@ -28440,6 +28782,9 @@
       <c r="D909" t="s">
         <v>914</v>
       </c>
+      <c r="E909" t="s">
+        <v>913</v>
+      </c>
       <c r="F909" t="b">
         <v>1</v>
       </c>
@@ -28460,6 +28805,9 @@
       <c r="D910" t="s">
         <v>915</v>
       </c>
+      <c r="E910" t="s">
+        <v>913</v>
+      </c>
       <c r="F910" t="b">
         <v>1</v>
       </c>
@@ -28620,6 +28968,9 @@
       <c r="D918" t="s">
         <v>2883</v>
       </c>
+      <c r="E918" t="s">
+        <v>955</v>
+      </c>
       <c r="F918" t="b">
         <v>0</v>
       </c>
@@ -28760,6 +29111,9 @@
       <c r="D925" t="s">
         <v>930</v>
       </c>
+      <c r="E925" t="s">
+        <v>929</v>
+      </c>
       <c r="F925" t="b">
         <v>1</v>
       </c>
@@ -28820,6 +29174,9 @@
       <c r="D928" t="s">
         <v>933</v>
       </c>
+      <c r="E928" t="s">
+        <v>929</v>
+      </c>
       <c r="F928" t="b">
         <v>1</v>
       </c>
@@ -28880,6 +29237,9 @@
       <c r="D931" t="s">
         <v>936</v>
       </c>
+      <c r="E931" t="s">
+        <v>935</v>
+      </c>
       <c r="F931" t="b">
         <v>1</v>
       </c>
@@ -28900,6 +29260,9 @@
       <c r="D932" t="s">
         <v>937</v>
       </c>
+      <c r="E932" t="s">
+        <v>935</v>
+      </c>
       <c r="F932" t="b">
         <v>1</v>
       </c>
@@ -28920,6 +29283,9 @@
       <c r="D933" t="s">
         <v>938</v>
       </c>
+      <c r="E933" t="s">
+        <v>935</v>
+      </c>
       <c r="F933" t="b">
         <v>1</v>
       </c>
@@ -29020,6 +29386,9 @@
       <c r="D938" t="s">
         <v>943</v>
       </c>
+      <c r="E938" t="s">
+        <v>942</v>
+      </c>
       <c r="F938" t="b">
         <v>1</v>
       </c>
@@ -29340,6 +29709,9 @@
       <c r="D954" t="s">
         <v>2894</v>
       </c>
+      <c r="E954" t="s">
+        <v>3262</v>
+      </c>
       <c r="F954" t="b">
         <v>1</v>
       </c>
@@ -30020,6 +30392,9 @@
       <c r="D988" t="s">
         <v>993</v>
       </c>
+      <c r="E988" t="s">
+        <v>992</v>
+      </c>
       <c r="F988" t="b">
         <v>1</v>
       </c>
@@ -30160,6 +30535,9 @@
       <c r="D995" t="s">
         <v>2906</v>
       </c>
+      <c r="E995" t="s">
+        <v>999</v>
+      </c>
       <c r="F995" t="b">
         <v>1</v>
       </c>
@@ -30600,6 +30978,9 @@
       <c r="D1017" t="s">
         <v>1022</v>
       </c>
+      <c r="E1017" t="s">
+        <v>3232</v>
+      </c>
       <c r="F1017" t="b">
         <v>0</v>
       </c>
@@ -30620,6 +31001,9 @@
       <c r="D1018" t="s">
         <v>1023</v>
       </c>
+      <c r="E1018" t="s">
+        <v>2522</v>
+      </c>
       <c r="F1018" t="b">
         <v>1</v>
       </c>
@@ -30760,6 +31144,9 @@
       <c r="D1025" t="s">
         <v>2908</v>
       </c>
+      <c r="E1025" t="s">
+        <v>3232</v>
+      </c>
       <c r="F1025" t="b">
         <v>0</v>
       </c>
@@ -31020,6 +31407,9 @@
       <c r="D1038" t="s">
         <v>1043</v>
       </c>
+      <c r="E1038" t="s">
+        <v>3232</v>
+      </c>
       <c r="F1038" t="b">
         <v>0</v>
       </c>
@@ -31040,6 +31430,9 @@
       <c r="D1039" t="s">
         <v>2910</v>
       </c>
+      <c r="E1039" t="s">
+        <v>1084</v>
+      </c>
       <c r="F1039" t="b">
         <v>0</v>
       </c>
@@ -31080,6 +31473,9 @@
       <c r="D1041" t="s">
         <v>1046</v>
       </c>
+      <c r="E1041" t="s">
+        <v>1084</v>
+      </c>
       <c r="F1041" t="b">
         <v>0</v>
       </c>
@@ -31260,6 +31656,9 @@
       <c r="D1050" t="s">
         <v>1055</v>
       </c>
+      <c r="E1050" t="s">
+        <v>3232</v>
+      </c>
       <c r="F1050" t="b">
         <v>1</v>
       </c>
@@ -31280,6 +31679,9 @@
       <c r="D1051" t="s">
         <v>1056</v>
       </c>
+      <c r="E1051" t="s">
+        <v>3232</v>
+      </c>
       <c r="F1051" t="b">
         <v>1</v>
       </c>
@@ -31600,6 +32002,9 @@
       <c r="D1067" t="s">
         <v>1072</v>
       </c>
+      <c r="E1067" t="s">
+        <v>1071</v>
+      </c>
       <c r="F1067" t="b">
         <v>1</v>
       </c>
@@ -31860,6 +32265,9 @@
       <c r="D1080" t="s">
         <v>1085</v>
       </c>
+      <c r="E1080" t="s">
+        <v>1084</v>
+      </c>
       <c r="F1080" t="b">
         <v>0</v>
       </c>
@@ -31880,6 +32288,9 @@
       <c r="D1081" t="s">
         <v>1086</v>
       </c>
+      <c r="E1081" t="s">
+        <v>1084</v>
+      </c>
       <c r="F1081" t="b">
         <v>0</v>
       </c>
@@ -32040,6 +32451,9 @@
       <c r="D1089" t="s">
         <v>2918</v>
       </c>
+      <c r="E1089" t="s">
+        <v>3263</v>
+      </c>
       <c r="F1089" t="b">
         <v>0</v>
       </c>
@@ -32180,6 +32594,9 @@
       <c r="D1096" t="s">
         <v>2919</v>
       </c>
+      <c r="E1096" t="s">
+        <v>3264</v>
+      </c>
       <c r="F1096" t="b">
         <v>0</v>
       </c>
@@ -32900,6 +33317,9 @@
       <c r="D1132" t="s">
         <v>1137</v>
       </c>
+      <c r="E1132" t="s">
+        <v>1136</v>
+      </c>
       <c r="F1132" t="b">
         <v>1</v>
       </c>
@@ -33560,6 +33980,9 @@
       <c r="D1165" t="s">
         <v>2928</v>
       </c>
+      <c r="E1165" t="s">
+        <v>992</v>
+      </c>
       <c r="F1165" t="b">
         <v>1</v>
       </c>
@@ -34500,6 +34923,9 @@
       <c r="D1212" t="s">
         <v>1217</v>
       </c>
+      <c r="E1212" t="s">
+        <v>1216</v>
+      </c>
       <c r="F1212" t="b">
         <v>1</v>
       </c>
@@ -34520,6 +34946,9 @@
       <c r="D1213" t="s">
         <v>1218</v>
       </c>
+      <c r="E1213" t="s">
+        <v>1216</v>
+      </c>
       <c r="F1213" t="b">
         <v>0</v>
       </c>
@@ -34700,6 +35129,9 @@
       <c r="D1222" t="s">
         <v>2943</v>
       </c>
+      <c r="E1222" t="s">
+        <v>3232</v>
+      </c>
       <c r="F1222" t="b">
         <v>1</v>
       </c>
@@ -35080,6 +35512,9 @@
       <c r="D1241" t="s">
         <v>2951</v>
       </c>
+      <c r="E1241" t="s">
+        <v>3265</v>
+      </c>
       <c r="F1241" t="b">
         <v>0</v>
       </c>
@@ -35220,6 +35655,9 @@
       <c r="D1248" t="s">
         <v>1253</v>
       </c>
+      <c r="E1248" t="s">
+        <v>3232</v>
+      </c>
       <c r="F1248" t="b">
         <v>1</v>
       </c>
@@ -35360,6 +35798,9 @@
       <c r="D1255" t="s">
         <v>2954</v>
       </c>
+      <c r="E1255" t="s">
+        <v>1259</v>
+      </c>
       <c r="F1255" t="b">
         <v>1</v>
       </c>
@@ -35380,6 +35821,9 @@
       <c r="D1256" t="s">
         <v>1261</v>
       </c>
+      <c r="E1256" t="s">
+        <v>1259</v>
+      </c>
       <c r="F1256" t="b">
         <v>1</v>
       </c>
@@ -35400,6 +35844,9 @@
       <c r="D1257" t="s">
         <v>1262</v>
       </c>
+      <c r="E1257" t="s">
+        <v>1259</v>
+      </c>
       <c r="F1257" t="b">
         <v>1</v>
       </c>
@@ -35420,6 +35867,9 @@
       <c r="D1258" t="s">
         <v>1263</v>
       </c>
+      <c r="E1258" t="s">
+        <v>1259</v>
+      </c>
       <c r="F1258" t="b">
         <v>1</v>
       </c>
@@ -35440,6 +35890,9 @@
       <c r="D1259" t="s">
         <v>2955</v>
       </c>
+      <c r="E1259" t="s">
+        <v>1259</v>
+      </c>
       <c r="F1259" t="b">
         <v>1</v>
       </c>
@@ -35460,6 +35913,9 @@
       <c r="D1260" t="s">
         <v>1265</v>
       </c>
+      <c r="E1260" t="s">
+        <v>1259</v>
+      </c>
       <c r="F1260" t="b">
         <v>1</v>
       </c>
@@ -35480,6 +35936,9 @@
       <c r="D1261" t="s">
         <v>1266</v>
       </c>
+      <c r="E1261" t="s">
+        <v>1259</v>
+      </c>
       <c r="F1261" t="b">
         <v>1</v>
       </c>
@@ -35880,6 +36339,9 @@
       <c r="D1281" t="s">
         <v>1286</v>
       </c>
+      <c r="E1281" t="s">
+        <v>3232</v>
+      </c>
       <c r="F1281" t="b">
         <v>0</v>
       </c>
@@ -36160,6 +36622,9 @@
       <c r="D1295" t="s">
         <v>1300</v>
       </c>
+      <c r="E1295" t="s">
+        <v>3266</v>
+      </c>
       <c r="F1295" t="b">
         <v>0</v>
       </c>
@@ -36480,6 +36945,9 @@
       <c r="D1311" t="s">
         <v>1316</v>
       </c>
+      <c r="E1311" t="s">
+        <v>1315</v>
+      </c>
       <c r="F1311" t="b">
         <v>1</v>
       </c>
@@ -36580,6 +37048,9 @@
       <c r="D1316" t="s">
         <v>2965</v>
       </c>
+      <c r="E1316" t="s">
+        <v>3267</v>
+      </c>
       <c r="F1316" t="b">
         <v>0</v>
       </c>
@@ -36600,6 +37071,9 @@
       <c r="D1317" t="s">
         <v>1322</v>
       </c>
+      <c r="E1317" t="s">
+        <v>3267</v>
+      </c>
       <c r="F1317" t="b">
         <v>1</v>
       </c>
@@ -36800,6 +37274,9 @@
       <c r="D1327" t="s">
         <v>1332</v>
       </c>
+      <c r="E1327" t="s">
+        <v>3232</v>
+      </c>
       <c r="F1327" t="b">
         <v>1</v>
       </c>
@@ -36900,6 +37377,9 @@
       <c r="D1332" t="s">
         <v>2968</v>
       </c>
+      <c r="E1332" t="s">
+        <v>1366</v>
+      </c>
       <c r="F1332" t="b">
         <v>0</v>
       </c>
@@ -37380,6 +37860,9 @@
       <c r="D1356" t="s">
         <v>1361</v>
       </c>
+      <c r="E1356" t="s">
+        <v>1360</v>
+      </c>
       <c r="F1356" t="b">
         <v>0</v>
       </c>
@@ -37560,6 +38043,9 @@
       <c r="D1365" t="s">
         <v>1370</v>
       </c>
+      <c r="E1365" t="s">
+        <v>3232</v>
+      </c>
       <c r="F1365" t="b">
         <v>1</v>
       </c>
@@ -37580,6 +38066,9 @@
       <c r="D1366" t="s">
         <v>1371</v>
       </c>
+      <c r="E1366" t="s">
+        <v>3232</v>
+      </c>
       <c r="F1366" t="b">
         <v>1</v>
       </c>
@@ -37600,6 +38089,9 @@
       <c r="D1367" t="s">
         <v>1372</v>
       </c>
+      <c r="E1367" t="s">
+        <v>3268</v>
+      </c>
       <c r="F1367" t="b">
         <v>0</v>
       </c>
@@ -37760,6 +38252,9 @@
       <c r="D1375" t="s">
         <v>1380</v>
       </c>
+      <c r="E1375" t="s">
+        <v>1379</v>
+      </c>
       <c r="F1375" t="b">
         <v>0</v>
       </c>
@@ -37840,6 +38335,9 @@
       <c r="D1379" t="s">
         <v>1384</v>
       </c>
+      <c r="E1379" t="s">
+        <v>1383</v>
+      </c>
       <c r="F1379" t="b">
         <v>1</v>
       </c>
@@ -38840,6 +39338,9 @@
       <c r="D1429" t="s">
         <v>1434</v>
       </c>
+      <c r="E1429" t="s">
+        <v>1433</v>
+      </c>
       <c r="F1429" t="b">
         <v>0</v>
       </c>
@@ -39660,6 +40161,9 @@
       <c r="D1470" t="s">
         <v>1475</v>
       </c>
+      <c r="E1470" t="s">
+        <v>3269</v>
+      </c>
       <c r="F1470" t="b">
         <v>0</v>
       </c>
@@ -39800,6 +40304,9 @@
       <c r="D1477" t="s">
         <v>1482</v>
       </c>
+      <c r="E1477" t="s">
+        <v>1483</v>
+      </c>
       <c r="F1477" t="b">
         <v>0</v>
       </c>
@@ -40340,6 +40847,9 @@
       <c r="D1504" t="s">
         <v>3004</v>
       </c>
+      <c r="E1504" t="s">
+        <v>1533</v>
+      </c>
       <c r="F1504" t="b">
         <v>0</v>
       </c>
@@ -40380,6 +40890,9 @@
       <c r="D1506" t="s">
         <v>1511</v>
       </c>
+      <c r="E1506" t="s">
+        <v>3270</v>
+      </c>
       <c r="F1506" t="b">
         <v>0</v>
       </c>
@@ -40800,6 +41313,9 @@
       <c r="D1527" t="s">
         <v>1532</v>
       </c>
+      <c r="E1527" t="s">
+        <v>1529</v>
+      </c>
       <c r="F1527" t="b">
         <v>0</v>
       </c>
@@ -40840,6 +41356,9 @@
       <c r="D1529" t="s">
         <v>1534</v>
       </c>
+      <c r="E1529" t="s">
+        <v>1533</v>
+      </c>
       <c r="F1529" t="b">
         <v>1</v>
       </c>
@@ -40860,6 +41379,9 @@
       <c r="D1530" t="s">
         <v>1535</v>
       </c>
+      <c r="E1530" t="s">
+        <v>3268</v>
+      </c>
       <c r="F1530" t="b">
         <v>1</v>
       </c>
@@ -40980,6 +41502,9 @@
       <c r="D1536" t="s">
         <v>1541</v>
       </c>
+      <c r="E1536" t="s">
+        <v>3232</v>
+      </c>
       <c r="F1536" t="b">
         <v>1</v>
       </c>
@@ -41120,6 +41645,9 @@
       <c r="D1543" t="s">
         <v>3013</v>
       </c>
+      <c r="E1543" t="s">
+        <v>3271</v>
+      </c>
       <c r="F1543" t="b">
         <v>0</v>
       </c>
@@ -41360,6 +41888,9 @@
       <c r="D1555" t="s">
         <v>3015</v>
       </c>
+      <c r="E1555" t="s">
+        <v>3272</v>
+      </c>
       <c r="F1555" t="b">
         <v>0</v>
       </c>
@@ -41380,6 +41911,9 @@
       <c r="D1556" t="s">
         <v>3016</v>
       </c>
+      <c r="E1556" t="s">
+        <v>3273</v>
+      </c>
       <c r="F1556" t="b">
         <v>1</v>
       </c>
@@ -41520,6 +42054,9 @@
       <c r="D1563" t="s">
         <v>3019</v>
       </c>
+      <c r="E1563" t="s">
+        <v>3272</v>
+      </c>
       <c r="F1563" t="b">
         <v>0</v>
       </c>
@@ -41660,6 +42197,9 @@
       <c r="D1570" t="s">
         <v>1575</v>
       </c>
+      <c r="E1570" t="s">
+        <v>1574</v>
+      </c>
       <c r="F1570" t="b">
         <v>1</v>
       </c>
@@ -41700,6 +42240,9 @@
       <c r="D1572" t="s">
         <v>1577</v>
       </c>
+      <c r="E1572" t="s">
+        <v>3272</v>
+      </c>
       <c r="F1572" t="b">
         <v>0</v>
       </c>
@@ -42120,6 +42663,9 @@
       <c r="D1593" t="s">
         <v>1598</v>
       </c>
+      <c r="E1593" t="s">
+        <v>1597</v>
+      </c>
       <c r="F1593" t="b">
         <v>1</v>
       </c>
@@ -42280,6 +42826,9 @@
       <c r="D1601" t="s">
         <v>3030</v>
       </c>
+      <c r="E1601" t="s">
+        <v>1605</v>
+      </c>
       <c r="F1601" t="b">
         <v>1</v>
       </c>
@@ -43060,6 +43609,9 @@
       <c r="D1640" t="s">
         <v>3039</v>
       </c>
+      <c r="E1640" t="s">
+        <v>3232</v>
+      </c>
       <c r="F1640" t="b">
         <v>1</v>
       </c>
@@ -43080,6 +43632,9 @@
       <c r="D1641" t="s">
         <v>3040</v>
       </c>
+      <c r="E1641" t="s">
+        <v>3232</v>
+      </c>
       <c r="F1641" t="b">
         <v>0</v>
       </c>
@@ -43100,6 +43655,9 @@
       <c r="D1642" t="s">
         <v>3041</v>
       </c>
+      <c r="E1642" t="s">
+        <v>3232</v>
+      </c>
       <c r="F1642" t="b">
         <v>0</v>
       </c>
@@ -44100,6 +44658,9 @@
       <c r="D1692" t="s">
         <v>3054</v>
       </c>
+      <c r="E1692" t="s">
+        <v>3232</v>
+      </c>
       <c r="F1692" t="b">
         <v>1</v>
       </c>
@@ -44320,6 +44881,9 @@
       <c r="D1703" t="s">
         <v>1708</v>
       </c>
+      <c r="E1703" t="s">
+        <v>3232</v>
+      </c>
       <c r="F1703" t="b">
         <v>1</v>
       </c>
@@ -44480,6 +45044,9 @@
       <c r="D1711" t="s">
         <v>1716</v>
       </c>
+      <c r="E1711" t="s">
+        <v>3274</v>
+      </c>
       <c r="F1711" t="b">
         <v>0</v>
       </c>
@@ -44700,6 +45267,9 @@
       <c r="D1722" t="s">
         <v>1727</v>
       </c>
+      <c r="E1722" t="s">
+        <v>3232</v>
+      </c>
       <c r="F1722" t="b">
         <v>1</v>
       </c>
@@ -44720,6 +45290,9 @@
       <c r="D1723" t="s">
         <v>1728</v>
       </c>
+      <c r="E1723" t="s">
+        <v>3232</v>
+      </c>
       <c r="F1723" t="b">
         <v>1</v>
       </c>
@@ -44740,6 +45313,9 @@
       <c r="D1724" t="s">
         <v>1729</v>
       </c>
+      <c r="E1724" t="s">
+        <v>3232</v>
+      </c>
       <c r="F1724" t="b">
         <v>1</v>
       </c>
@@ -44760,6 +45336,9 @@
       <c r="D1725" t="s">
         <v>3062</v>
       </c>
+      <c r="E1725" t="s">
+        <v>3275</v>
+      </c>
       <c r="F1725" t="b">
         <v>0</v>
       </c>
@@ -44780,6 +45359,9 @@
       <c r="D1726" t="s">
         <v>1731</v>
       </c>
+      <c r="E1726" t="s">
+        <v>1732</v>
+      </c>
       <c r="F1726" t="b">
         <v>0</v>
       </c>
@@ -44980,6 +45562,9 @@
       <c r="D1736" t="s">
         <v>1741</v>
       </c>
+      <c r="E1736" t="s">
+        <v>227</v>
+      </c>
       <c r="F1736" t="b">
         <v>0</v>
       </c>
@@ -45120,6 +45705,9 @@
       <c r="D1743" t="s">
         <v>1748</v>
       </c>
+      <c r="E1743" t="s">
+        <v>1747</v>
+      </c>
       <c r="F1743" t="b">
         <v>0</v>
       </c>
@@ -45140,6 +45728,9 @@
       <c r="D1744" t="s">
         <v>1749</v>
       </c>
+      <c r="E1744" t="s">
+        <v>1747</v>
+      </c>
       <c r="F1744" t="b">
         <v>0</v>
       </c>
@@ -45280,6 +45871,9 @@
       <c r="D1751" t="s">
         <v>3067</v>
       </c>
+      <c r="E1751" t="s">
+        <v>3276</v>
+      </c>
       <c r="F1751" t="b">
         <v>0</v>
       </c>
@@ -45900,6 +46494,9 @@
       <c r="D1782" t="s">
         <v>3075</v>
       </c>
+      <c r="E1782" t="s">
+        <v>3277</v>
+      </c>
       <c r="F1782" t="b">
         <v>0</v>
       </c>
@@ -46340,6 +46937,9 @@
       <c r="D1804" t="s">
         <v>3079</v>
       </c>
+      <c r="E1804" t="s">
+        <v>3278</v>
+      </c>
       <c r="F1804" t="b">
         <v>0</v>
       </c>
@@ -46360,6 +46960,9 @@
       <c r="D1805" t="s">
         <v>1810</v>
       </c>
+      <c r="E1805" t="s">
+        <v>3278</v>
+      </c>
       <c r="F1805" t="b">
         <v>0</v>
       </c>
@@ -46520,6 +47123,9 @@
       <c r="D1813" t="s">
         <v>3081</v>
       </c>
+      <c r="E1813" t="s">
+        <v>1818</v>
+      </c>
       <c r="F1813" t="b">
         <v>0</v>
       </c>
@@ -46540,6 +47146,9 @@
       <c r="D1814" t="s">
         <v>1819</v>
       </c>
+      <c r="E1814" t="s">
+        <v>1818</v>
+      </c>
       <c r="F1814" t="b">
         <v>1</v>
       </c>
@@ -46600,6 +47209,9 @@
       <c r="D1817" t="s">
         <v>1822</v>
       </c>
+      <c r="E1817" t="s">
+        <v>3232</v>
+      </c>
       <c r="F1817" t="b">
         <v>1</v>
       </c>
@@ -46980,6 +47592,9 @@
       <c r="D1836" t="s">
         <v>1841</v>
       </c>
+      <c r="E1836" t="s">
+        <v>1763</v>
+      </c>
       <c r="F1836" t="b">
         <v>0</v>
       </c>
@@ -47180,6 +47795,9 @@
       <c r="D1846" t="s">
         <v>1851</v>
       </c>
+      <c r="E1846" t="s">
+        <v>3279</v>
+      </c>
       <c r="F1846" t="b">
         <v>0</v>
       </c>
@@ -47240,6 +47858,9 @@
       <c r="D1849" t="s">
         <v>1854</v>
       </c>
+      <c r="E1849" t="s">
+        <v>1853</v>
+      </c>
       <c r="F1849" t="b">
         <v>1</v>
       </c>
@@ -48000,6 +48621,9 @@
       <c r="D1887" t="s">
         <v>1892</v>
       </c>
+      <c r="E1887" t="s">
+        <v>3280</v>
+      </c>
       <c r="F1887" t="b">
         <v>1</v>
       </c>
@@ -48240,6 +48864,9 @@
       <c r="D1899" t="s">
         <v>1904</v>
       </c>
+      <c r="E1899" t="s">
+        <v>1903</v>
+      </c>
       <c r="F1899" t="b">
         <v>1</v>
       </c>
@@ -48560,6 +49187,9 @@
       <c r="D1915" t="s">
         <v>1920</v>
       </c>
+      <c r="E1915" t="s">
+        <v>1919</v>
+      </c>
       <c r="F1915" t="b">
         <v>0</v>
       </c>
@@ -48640,6 +49270,9 @@
       <c r="D1919" t="s">
         <v>3102</v>
       </c>
+      <c r="E1919" t="s">
+        <v>3281</v>
+      </c>
       <c r="F1919" t="b">
         <v>0</v>
       </c>
@@ -49180,6 +49813,9 @@
       <c r="D1946" t="s">
         <v>3109</v>
       </c>
+      <c r="E1946" t="s">
+        <v>3232</v>
+      </c>
       <c r="F1946" t="b">
         <v>1</v>
       </c>
@@ -49220,6 +49856,9 @@
       <c r="D1948" t="s">
         <v>1953</v>
       </c>
+      <c r="E1948" t="s">
+        <v>3232</v>
+      </c>
       <c r="F1948" t="b">
         <v>1</v>
       </c>
@@ -49260,6 +49899,9 @@
       <c r="D1950" t="s">
         <v>1955</v>
       </c>
+      <c r="E1950" t="s">
+        <v>3232</v>
+      </c>
       <c r="F1950" t="b">
         <v>0</v>
       </c>
@@ -49280,6 +49922,9 @@
       <c r="D1951" t="s">
         <v>3111</v>
       </c>
+      <c r="E1951" t="s">
+        <v>3232</v>
+      </c>
       <c r="F1951" t="b">
         <v>0</v>
       </c>
@@ -49300,6 +49945,9 @@
       <c r="D1952" t="s">
         <v>1957</v>
       </c>
+      <c r="E1952" t="s">
+        <v>3232</v>
+      </c>
       <c r="F1952" t="b">
         <v>1</v>
       </c>
@@ -51080,6 +51728,9 @@
       <c r="D2041" t="s">
         <v>2046</v>
       </c>
+      <c r="E2041" t="s">
+        <v>2045</v>
+      </c>
       <c r="F2041" t="b">
         <v>1</v>
       </c>
@@ -51140,6 +51791,9 @@
       <c r="D2044" t="s">
         <v>3135</v>
       </c>
+      <c r="E2044" t="s">
+        <v>3232</v>
+      </c>
       <c r="F2044" t="b">
         <v>0</v>
       </c>
@@ -52180,6 +52834,9 @@
       <c r="D2096" t="s">
         <v>2101</v>
       </c>
+      <c r="E2096" t="s">
+        <v>3232</v>
+      </c>
       <c r="F2096" t="b">
         <v>0</v>
       </c>
@@ -52780,6 +53437,9 @@
       <c r="D2126" t="s">
         <v>2131</v>
       </c>
+      <c r="E2126" t="s">
+        <v>3232</v>
+      </c>
       <c r="F2126" t="b">
         <v>0</v>
       </c>
@@ -53320,6 +53980,9 @@
       <c r="D2153" t="s">
         <v>2158</v>
       </c>
+      <c r="E2153" t="s">
+        <v>2153</v>
+      </c>
       <c r="F2153" t="b">
         <v>1</v>
       </c>
@@ -53500,6 +54163,9 @@
       <c r="D2162" t="s">
         <v>3150</v>
       </c>
+      <c r="E2162" t="s">
+        <v>227</v>
+      </c>
       <c r="F2162" t="b">
         <v>1</v>
       </c>
@@ -53980,6 +54646,9 @@
       <c r="D2186" t="s">
         <v>2191</v>
       </c>
+      <c r="E2186" t="s">
+        <v>2190</v>
+      </c>
       <c r="F2186" t="b">
         <v>1</v>
       </c>
@@ -54040,6 +54709,9 @@
       <c r="D2189" t="s">
         <v>3161</v>
       </c>
+      <c r="E2189" t="s">
+        <v>2193</v>
+      </c>
       <c r="F2189" t="b">
         <v>0</v>
       </c>
@@ -54400,6 +55072,9 @@
       <c r="D2207" t="s">
         <v>3165</v>
       </c>
+      <c r="E2207" t="s">
+        <v>3232</v>
+      </c>
       <c r="F2207" t="b">
         <v>1</v>
       </c>
@@ -54420,6 +55095,9 @@
       <c r="D2208" t="s">
         <v>3166</v>
       </c>
+      <c r="E2208" t="s">
+        <v>74</v>
+      </c>
       <c r="F2208" t="b">
         <v>0</v>
       </c>
@@ -54620,6 +55298,9 @@
       <c r="D2218" t="s">
         <v>2223</v>
       </c>
+      <c r="E2218" t="s">
+        <v>3232</v>
+      </c>
       <c r="F2218" t="b">
         <v>1</v>
       </c>
@@ -55080,6 +55761,9 @@
       <c r="D2241" t="s">
         <v>2246</v>
       </c>
+      <c r="E2241" t="s">
+        <v>2245</v>
+      </c>
       <c r="F2241" t="b">
         <v>1</v>
       </c>
@@ -55200,6 +55884,9 @@
       <c r="D2247" t="s">
         <v>2252</v>
       </c>
+      <c r="E2247" t="s">
+        <v>3282</v>
+      </c>
       <c r="F2247" t="b">
         <v>0</v>
       </c>
@@ -55260,6 +55947,9 @@
       <c r="D2250" t="s">
         <v>3173</v>
       </c>
+      <c r="E2250" t="s">
+        <v>3283</v>
+      </c>
       <c r="F2250" t="b">
         <v>0</v>
       </c>
@@ -56220,6 +56910,9 @@
       <c r="D2298" t="s">
         <v>2303</v>
       </c>
+      <c r="E2298" t="s">
+        <v>3232</v>
+      </c>
       <c r="F2298" t="b">
         <v>1</v>
       </c>
@@ -56700,6 +57393,9 @@
       <c r="D2322" t="s">
         <v>2327</v>
       </c>
+      <c r="E2322" t="s">
+        <v>3232</v>
+      </c>
       <c r="F2322" t="b">
         <v>1</v>
       </c>
@@ -56880,6 +57576,9 @@
       <c r="D2331" t="s">
         <v>3182</v>
       </c>
+      <c r="E2331" t="s">
+        <v>3284</v>
+      </c>
       <c r="F2331" t="b">
         <v>1</v>
       </c>
@@ -56920,6 +57619,9 @@
       <c r="D2333" t="s">
         <v>3183</v>
       </c>
+      <c r="E2333" t="s">
+        <v>2402</v>
+      </c>
       <c r="F2333" t="b">
         <v>0</v>
       </c>
@@ -57280,6 +57982,9 @@
       <c r="D2351" t="s">
         <v>3187</v>
       </c>
+      <c r="E2351" t="s">
+        <v>2435</v>
+      </c>
       <c r="F2351" t="b">
         <v>0</v>
       </c>
@@ -57320,6 +58025,9 @@
       <c r="D2353" t="s">
         <v>3188</v>
       </c>
+      <c r="E2353" t="s">
+        <v>3232</v>
+      </c>
       <c r="F2353" t="b">
         <v>0</v>
       </c>
@@ -57540,6 +58248,9 @@
       <c r="D2364" t="s">
         <v>3192</v>
       </c>
+      <c r="E2364" t="s">
+        <v>992</v>
+      </c>
       <c r="F2364" t="b">
         <v>1</v>
       </c>
@@ -57720,6 +58431,9 @@
       <c r="D2373" t="s">
         <v>3193</v>
       </c>
+      <c r="E2373" t="s">
+        <v>3232</v>
+      </c>
       <c r="F2373" t="b">
         <v>1</v>
       </c>
@@ -58060,6 +58774,9 @@
       <c r="D2390" t="s">
         <v>2395</v>
       </c>
+      <c r="E2390" t="s">
+        <v>227</v>
+      </c>
       <c r="F2390" t="b">
         <v>1</v>
       </c>
@@ -58080,6 +58797,9 @@
       <c r="D2391" t="s">
         <v>2396</v>
       </c>
+      <c r="E2391" t="s">
+        <v>3285</v>
+      </c>
       <c r="F2391" t="b">
         <v>1</v>
       </c>
@@ -58420,6 +59140,9 @@
       <c r="D2408" t="s">
         <v>3199</v>
       </c>
+      <c r="E2408" t="s">
+        <v>3286</v>
+      </c>
       <c r="F2408" t="b">
         <v>0</v>
       </c>
@@ -58540,6 +59263,9 @@
       <c r="D2414" t="s">
         <v>2419</v>
       </c>
+      <c r="E2414" t="s">
+        <v>935</v>
+      </c>
       <c r="F2414" t="b">
         <v>1</v>
       </c>
@@ -58600,6 +59326,9 @@
       <c r="D2417" t="s">
         <v>3202</v>
       </c>
+      <c r="E2417" t="s">
+        <v>3287</v>
+      </c>
       <c r="F2417" t="b">
         <v>0</v>
       </c>
@@ -58620,6 +59349,9 @@
       <c r="D2418" t="s">
         <v>3203</v>
       </c>
+      <c r="E2418" t="s">
+        <v>3288</v>
+      </c>
       <c r="F2418" t="b">
         <v>0</v>
       </c>
@@ -58660,6 +59392,9 @@
       <c r="D2420" t="s">
         <v>3204</v>
       </c>
+      <c r="E2420" t="s">
+        <v>3289</v>
+      </c>
       <c r="F2420" t="b">
         <v>1</v>
       </c>
@@ -58680,6 +59415,9 @@
       <c r="D2421" t="s">
         <v>2426</v>
       </c>
+      <c r="E2421" t="s">
+        <v>227</v>
+      </c>
       <c r="F2421" t="b">
         <v>1</v>
       </c>
@@ -58880,6 +59618,9 @@
       <c r="D2431" t="s">
         <v>2436</v>
       </c>
+      <c r="E2431" t="s">
+        <v>2435</v>
+      </c>
       <c r="F2431" t="b">
         <v>0</v>
       </c>
@@ -58900,6 +59641,9 @@
       <c r="D2432" t="s">
         <v>2437</v>
       </c>
+      <c r="E2432" t="s">
+        <v>2435</v>
+      </c>
       <c r="F2432" t="b">
         <v>0</v>
       </c>
@@ -58920,6 +59664,9 @@
       <c r="D2433" t="s">
         <v>2438</v>
       </c>
+      <c r="E2433" t="s">
+        <v>2435</v>
+      </c>
       <c r="F2433" t="b">
         <v>1</v>
       </c>
@@ -59080,6 +59827,9 @@
       <c r="D2441" t="s">
         <v>2446</v>
       </c>
+      <c r="E2441" t="s">
+        <v>2445</v>
+      </c>
       <c r="F2441" t="b">
         <v>1</v>
       </c>
@@ -59140,6 +59890,9 @@
       <c r="D2444" t="s">
         <v>2449</v>
       </c>
+      <c r="E2444" t="s">
+        <v>2480</v>
+      </c>
       <c r="F2444" t="b">
         <v>0</v>
       </c>
@@ -59160,6 +59913,9 @@
       <c r="D2445" t="s">
         <v>2450</v>
       </c>
+      <c r="E2445" t="s">
+        <v>2439</v>
+      </c>
       <c r="F2445" t="b">
         <v>0</v>
       </c>
@@ -59180,6 +59936,9 @@
       <c r="D2446" t="s">
         <v>3214</v>
       </c>
+      <c r="E2446" t="s">
+        <v>3290</v>
+      </c>
       <c r="F2446" t="b">
         <v>0</v>
       </c>
@@ -60220,6 +60979,9 @@
       <c r="D2498" t="s">
         <v>2503</v>
       </c>
+      <c r="E2498" t="s">
+        <v>2502</v>
+      </c>
       <c r="F2498" t="b">
         <v>0</v>
       </c>
@@ -60340,6 +61102,9 @@
       <c r="D2504" t="s">
         <v>3223</v>
       </c>
+      <c r="E2504" t="s">
+        <v>3232</v>
+      </c>
       <c r="F2504" t="b">
         <v>1</v>
       </c>
@@ -60380,6 +61145,9 @@
       <c r="D2506" t="s">
         <v>3224</v>
       </c>
+      <c r="E2506" t="s">
+        <v>3232</v>
+      </c>
       <c r="F2506" t="b">
         <v>1</v>
       </c>
@@ -60400,6 +61168,9 @@
       <c r="D2507" t="s">
         <v>3225</v>
       </c>
+      <c r="E2507" t="s">
+        <v>2522</v>
+      </c>
       <c r="F2507" t="b">
         <v>0</v>
       </c>
@@ -60460,6 +61231,9 @@
       <c r="D2510" t="s">
         <v>3227</v>
       </c>
+      <c r="E2510" t="s">
+        <v>3291</v>
+      </c>
       <c r="F2510" t="b">
         <v>0</v>
       </c>
@@ -60500,6 +61274,9 @@
       <c r="D2512" t="s">
         <v>2517</v>
       </c>
+      <c r="E2512" t="s">
+        <v>2516</v>
+      </c>
       <c r="F2512" t="b">
         <v>1</v>
       </c>
@@ -60560,6 +61337,9 @@
       <c r="D2515" t="s">
         <v>3229</v>
       </c>
+      <c r="E2515" t="s">
+        <v>2522</v>
+      </c>
       <c r="F2515" t="b">
         <v>0</v>
       </c>
@@ -60620,6 +61400,9 @@
       <c r="D2518" t="s">
         <v>2523</v>
       </c>
+      <c r="E2518" t="s">
+        <v>2522</v>
+      </c>
       <c r="F2518" t="b">
         <v>1</v>
       </c>
@@ -60640,6 +61423,9 @@
       <c r="D2519" t="s">
         <v>2524</v>
       </c>
+      <c r="E2519" t="s">
+        <v>2522</v>
+      </c>
       <c r="F2519" t="b">
         <v>1</v>
       </c>
@@ -60660,6 +61446,9 @@
       <c r="D2520" t="s">
         <v>2525</v>
       </c>
+      <c r="E2520" t="s">
+        <v>3232</v>
+      </c>
       <c r="F2520" t="b">
         <v>1</v>
       </c>
@@ -60819,6 +61608,9 @@
       </c>
       <c r="D2528" t="s">
         <v>2533</v>
+      </c>
+      <c r="E2528" t="s">
+        <v>3232</v>
       </c>
       <c r="F2528" t="b">
         <v>1</v>

</xml_diff>